<commit_message>
Nka and Lka additions to release version
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/excelTemplates/rjkam_template.xlsx
+++ b/src/main/webapp/resources/excelTemplates/rjkam_template.xlsx
@@ -50,7 +50,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="AT12")</t>
+jx:area(lastCell="AU15")</t>
         </r>
       </text>
     </comment>
@@ -74,7 +74,31 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="rjkamReportItemList", var="rjkamReportItem", lastCell="AT12" multisheet="sheetNames")</t>
+jx:each(items="rjkamReportItemList" var="rjkamGroup" groupBy="name" groupOrder="asc" lastCell="AU15" multisheet="sheetNames" )</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="rjkamGroup.items" var="rjkam" lastCell="AU12")</t>
         </r>
       </text>
     </comment>
@@ -100,7 +124,7 @@
             <charset val="204"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="rjkamReportItem.reportItemList" groupBy="nkaId" groupOrder="asc" lastCell="AT12")</t>
+jx:each(items="rjkam.reportItemList" var="repGroup" groupBy="nkaId" groupOrder="asc" lastCell="AU12")</t>
         </r>
       </text>
     </comment>
@@ -125,7 +149,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="_group.items" var="reportItem" lastCell="AT12")</t>
+jx:each(items="repGroup.items" var="reportItem" lastCell="AU12")</t>
         </r>
       </text>
     </comment>
@@ -134,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>ТС / Адрес</t>
   </si>
@@ -211,12 +235,6 @@
     <t>ЦП / ЗП</t>
   </si>
   <si>
-    <t>${rjkamReportItem.name}</t>
-  </si>
-  <si>
-    <t>${_group.item.nkaName}</t>
-  </si>
-  <si>
     <t>${reportItem.type}</t>
   </si>
   <si>
@@ -298,12 +316,6 @@
     <t>Код</t>
   </si>
   <si>
-    <t>${rjkamReportItem.id}</t>
-  </si>
-  <si>
-    <t>${reportItem.nkaId}</t>
-  </si>
-  <si>
     <t>${reportItem.clientName}</t>
   </si>
   <si>
@@ -332,6 +344,24 @@
   </si>
   <si>
     <t>${reportItem.sDmNa}</t>
+  </si>
+  <si>
+    <t>${rjkamGroup.item.id}</t>
+  </si>
+  <si>
+    <t>${rjkamGroup.item.name}</t>
+  </si>
+  <si>
+    <t>${repGroup.item.nkaId}</t>
+  </si>
+  <si>
+    <t>${repGroup.item.nkaName}</t>
+  </si>
+  <si>
+    <t>Дата послед. фото</t>
+  </si>
+  <si>
+    <t>${reportItem.lastPhotoDate}</t>
   </si>
 </sst>
 </file>
@@ -421,7 +451,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +506,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -656,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -769,103 +805,106 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1186,14 +1225,14 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AT12"/>
+  <dimension ref="A1:AU12"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="AJ21" sqref="AJ21"/>
       <selection pane="topRight" activeCell="AJ21" sqref="AJ21"/>
       <selection pane="bottomLeft" activeCell="AJ21" sqref="AJ21"/>
-      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1206,36 +1245,34 @@
     <col min="6" max="6" width="15" style="2" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="43.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="6" style="27" customWidth="1"/>
-    <col min="9" max="11" width="6" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="6" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="6" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="6" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="20" width="6" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="6" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="25" width="6" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="6" style="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="6" style="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="6" style="1" customWidth="1"/>
-    <col min="30" max="30" width="6" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="32" width="5.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="5.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="36" width="7.42578125" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="7.42578125" style="10" customWidth="1" collapsed="1"/>
-    <col min="38" max="40" width="7.42578125" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="6" style="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="6" style="1" customWidth="1"/>
-    <col min="43" max="45" width="6" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="6" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="11" width="6" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="6" style="1" customWidth="1"/>
+    <col min="13" max="15" width="6" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="6" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="20" width="6" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="6" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="25" width="6" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="6" style="1" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="29" width="6" style="1" customWidth="1"/>
+    <col min="30" max="30" width="6" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="32" width="5.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="5.85546875" style="1" customWidth="1"/>
+    <col min="34" max="36" width="7.42578125" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="7.42578125" style="10" customWidth="1"/>
+    <col min="38" max="40" width="7.42578125" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="42" width="6" style="1" customWidth="1"/>
+    <col min="43" max="45" width="6" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="6" style="1" customWidth="1"/>
     <col min="47" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F2" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>20</v>
@@ -1249,12 +1286,12 @@
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
     </row>
-    <row r="3" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="H3" s="24"/>
       <c r="AH3" s="1"/>
@@ -1265,8 +1302,8 @@
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
     </row>
-    <row r="5" spans="1:46" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+    <row r="5" spans="1:47" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="17"/>
@@ -1274,270 +1311,276 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="19"/>
-      <c r="G5" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="65" t="s">
+      <c r="G5" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="65"/>
-      <c r="Z5" s="65"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="65"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="65"/>
-      <c r="AH5" s="65"/>
-      <c r="AI5" s="65"/>
-      <c r="AJ5" s="65"/>
-      <c r="AK5" s="65"/>
-      <c r="AL5" s="65"/>
-      <c r="AM5" s="65"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="65"/>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="65"/>
-      <c r="AR5" s="65"/>
-      <c r="AS5" s="65"/>
-      <c r="AT5" s="65"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43"/>
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="43"/>
+      <c r="AJ5" s="43"/>
+      <c r="AK5" s="43"/>
+      <c r="AL5" s="43"/>
+      <c r="AM5" s="43"/>
+      <c r="AN5" s="43"/>
+      <c r="AO5" s="43"/>
+      <c r="AP5" s="43"/>
+      <c r="AQ5" s="43"/>
+      <c r="AR5" s="43"/>
+      <c r="AS5" s="43"/>
+      <c r="AT5" s="43"/>
+      <c r="AU5" s="38" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
+    <row r="6" spans="1:47" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="40" t="s">
+      <c r="G6" s="71"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
-      <c r="X6" s="40"/>
-      <c r="Y6" s="40"/>
-      <c r="Z6" s="40"/>
-      <c r="AA6" s="40"/>
-      <c r="AB6" s="40"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="46"/>
+      <c r="Z6" s="46"/>
+      <c r="AA6" s="46"/>
+      <c r="AB6" s="46"/>
       <c r="AC6" s="31"/>
-      <c r="AD6" s="47" t="s">
+      <c r="AD6" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="AE6" s="48"/>
-      <c r="AF6" s="48"/>
-      <c r="AG6" s="49"/>
-      <c r="AH6" s="68" t="s">
+      <c r="AE6" s="65"/>
+      <c r="AF6" s="65"/>
+      <c r="AG6" s="66"/>
+      <c r="AH6" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AI6" s="69"/>
-      <c r="AJ6" s="69"/>
-      <c r="AK6" s="69"/>
-      <c r="AL6" s="69"/>
-      <c r="AM6" s="69"/>
-      <c r="AN6" s="69"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="69"/>
-      <c r="AQ6" s="69"/>
-      <c r="AR6" s="69"/>
-      <c r="AS6" s="69"/>
-      <c r="AT6" s="70"/>
+      <c r="AI6" s="57"/>
+      <c r="AJ6" s="57"/>
+      <c r="AK6" s="57"/>
+      <c r="AL6" s="57"/>
+      <c r="AM6" s="57"/>
+      <c r="AN6" s="57"/>
+      <c r="AO6" s="57"/>
+      <c r="AP6" s="57"/>
+      <c r="AQ6" s="57"/>
+      <c r="AR6" s="57"/>
+      <c r="AS6" s="57"/>
+      <c r="AT6" s="58"/>
+      <c r="AU6" s="38"/>
     </row>
-    <row r="7" spans="1:46" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
-      <c r="B7" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="58" t="s">
+    <row r="7" spans="1:47" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="44"/>
+      <c r="I7" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="66"/>
-      <c r="I7" s="40" t="s">
+      <c r="AD7" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="67"/>
+      <c r="AH7" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI7" s="48"/>
+      <c r="AJ7" s="48"/>
+      <c r="AK7" s="48"/>
+      <c r="AL7" s="48"/>
+      <c r="AM7" s="48"/>
+      <c r="AN7" s="48"/>
+      <c r="AO7" s="48"/>
+      <c r="AP7" s="49"/>
+      <c r="AQ7" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR7" s="48"/>
+      <c r="AS7" s="48"/>
+      <c r="AT7" s="49"/>
+      <c r="AU7" s="38"/>
+    </row>
+    <row r="8" spans="1:47" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="54"/>
+      <c r="V8" s="55"/>
+      <c r="W8" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="X8" s="54"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="54"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC8" s="62"/>
+      <c r="AD8" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF8" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG8" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40" t="s">
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
-      <c r="X7" s="40"/>
-      <c r="Y7" s="40"/>
-      <c r="Z7" s="40"/>
-      <c r="AA7" s="40"/>
-      <c r="AB7" s="40"/>
-      <c r="AC7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD7" s="50" t="s">
+      <c r="AM8" s="48"/>
+      <c r="AN8" s="48"/>
+      <c r="AO8" s="49"/>
+      <c r="AP8" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="AE7" s="50"/>
-      <c r="AF7" s="50"/>
-      <c r="AG7" s="50"/>
-      <c r="AH7" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI7" s="56"/>
-      <c r="AJ7" s="56"/>
-      <c r="AK7" s="56"/>
-      <c r="AL7" s="56"/>
-      <c r="AM7" s="56"/>
-      <c r="AN7" s="56"/>
-      <c r="AO7" s="56"/>
-      <c r="AP7" s="57"/>
-      <c r="AQ7" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="AR7" s="56"/>
-      <c r="AS7" s="56"/>
-      <c r="AT7" s="57"/>
+      <c r="AR8" s="48"/>
+      <c r="AS8" s="48"/>
+      <c r="AT8" s="49"/>
+      <c r="AU8" s="38"/>
     </row>
-    <row r="8" spans="1:46" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="45"/>
-      <c r="AA8" s="46"/>
-      <c r="AB8" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE8" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF8" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG8" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH8" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI8" s="56"/>
-      <c r="AJ8" s="56"/>
-      <c r="AK8" s="57"/>
-      <c r="AL8" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM8" s="56"/>
-      <c r="AN8" s="56"/>
-      <c r="AO8" s="57"/>
-      <c r="AP8" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ8" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="AR8" s="56"/>
-      <c r="AS8" s="56"/>
-      <c r="AT8" s="57"/>
-    </row>
-    <row r="9" spans="1:46" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
+    <row r="9" spans="1:47" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
       <c r="M9" s="16" t="s">
         <v>11</v>
       </c>
@@ -1583,12 +1626,12 @@
       <c r="AA9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="AB9" s="40"/>
+      <c r="AB9" s="46"/>
       <c r="AC9" s="63"/>
-      <c r="AD9" s="52"/>
-      <c r="AE9" s="52"/>
-      <c r="AF9" s="52"/>
-      <c r="AG9" s="52"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="69"/>
       <c r="AH9" s="30" t="s">
         <v>2</v>
       </c>
@@ -1599,7 +1642,7 @@
         <v>14</v>
       </c>
       <c r="AK9" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AL9" s="30" t="s">
         <v>2</v>
@@ -1611,9 +1654,9 @@
         <v>14</v>
       </c>
       <c r="AO9" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP9" s="54"/>
+        <v>50</v>
+      </c>
+      <c r="AP9" s="60"/>
       <c r="AQ9" s="30" t="s">
         <v>2</v>
       </c>
@@ -1624,10 +1667,11 @@
         <v>14</v>
       </c>
       <c r="AT9" s="30" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="AU9" s="38"/>
     </row>
-    <row r="10" spans="1:46" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1784,14 +1828,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="AU10" s="7"/>
     </row>
-    <row r="11" spans="1:46" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D11" s="14">
         <f>COUNTA(D12)</f>
@@ -1800,7 +1845,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="4">
@@ -1946,86 +1991,87 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU11" s="4"/>
     </row>
-    <row r="12" spans="1:46" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="H12" s="29"/>
       <c r="I12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="L12" s="6">
         <f>SUM(I12:K12)</f>
         <v>0</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P12" s="6">
         <f>SUM(M12:O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T12" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T12" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="U12" s="6">
         <f>SUM(R12:T12)</f>
         <v>0</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="W12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="X12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="X12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y12" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="Z12" s="6">
         <f>SUM(W12:Y12)</f>
         <v>0</v>
       </c>
       <c r="AA12" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AB12" s="6">
         <f>SUM(P12,U12,Z12)</f>
@@ -2036,39 +2082,39 @@
         <v>0</v>
       </c>
       <c r="AD12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF12" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="AE12" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF12" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="AG12" s="6">
         <f>SUM(AD12:AF12)</f>
         <v>0</v>
       </c>
       <c r="AH12" s="34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AI12" s="34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AJ12" s="34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AK12" s="6">
         <f>SUM(AH12:AJ12)</f>
         <v>0</v>
       </c>
       <c r="AL12" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AM12" s="34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AN12" s="34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AO12" s="6">
         <f>SUM(AL12:AN12)</f>
@@ -2079,21 +2125,45 @@
         <v>0</v>
       </c>
       <c r="AQ12" s="34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AR12" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AS12" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AT12" s="6">
         <f>SUM(AQ12:AS12)</f>
         <v>0</v>
       </c>
+      <c r="AU12" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M7:AB7"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AD7:AG7"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AE8:AE9"/>
+    <mergeCell ref="AF8:AF9"/>
+    <mergeCell ref="AG8:AG9"/>
+    <mergeCell ref="AH8:AK8"/>
+    <mergeCell ref="AP8:AP9"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="AC7:AC9"/>
+    <mergeCell ref="AU5:AU9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="B7:B9"/>
@@ -2109,26 +2179,6 @@
     <mergeCell ref="W8:AA8"/>
     <mergeCell ref="R8:V8"/>
     <mergeCell ref="AH6:AT6"/>
-    <mergeCell ref="AH8:AK8"/>
-    <mergeCell ref="AP8:AP9"/>
-    <mergeCell ref="AL8:AO8"/>
-    <mergeCell ref="AQ8:AT8"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="AC7:AC9"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD7:AG7"/>
-    <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="AE8:AE9"/>
-    <mergeCell ref="AF8:AF9"/>
-    <mergeCell ref="AG8:AG9"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M7:AB7"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>

</xml_diff>